<commit_message>
Updated test "VerReq_addSmartFormItem_PerformCheckOut" by reading RFQ value
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerReq_AddSmartFormItem_PerformCheckOut.xlsx
+++ b/src/test/resources/datasheets/VerReq_AddSmartFormItem_PerformCheckOut.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16335" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="AddSmartFormItem" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -440,7 +441,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>